<commit_message>
Ponowna optymalizacja wszystkich 15 przypadków, dodanie folderu New_figures z nowymi przebiegami, aktualizacja sprawozdania o wprowadzenie nowych wartości nastaw i wartości wskaźniaka jakości, aktualizacja pliku SAIE_nastawy.xlsx
</commit_message>
<xml_diff>
--- a/SAIE_nastawy.xlsx
+++ b/SAIE_nastawy.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Rubak\Documents\SAIE\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9525"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9528"/>
   </bookViews>
   <sheets>
     <sheet name="Zakłócenie Z1, pierwszy sygnał" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="16">
   <si>
     <t>r</t>
   </si>
@@ -158,7 +163,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -191,9 +196,16 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="60% - akcent 1" xfId="1" builtinId="32"/>
+    <cellStyle name="60% — akcent 1" xfId="1" builtinId="32"/>
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -464,7 +476,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -472,27 +484,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M52"/>
+  <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23:O23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" customWidth="1"/>
-    <col min="12" max="12" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" customWidth="1"/>
+    <col min="12" max="12" width="20.5546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -530,7 +542,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:13" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -568,7 +580,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:13" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -606,7 +618,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:13" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -644,7 +656,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:13" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -677,7 +689,7 @@
       </c>
       <c r="L5" s="10"/>
     </row>
-    <row r="6" spans="1:13" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -710,7 +722,7 @@
       </c>
       <c r="L6" s="10"/>
     </row>
-    <row r="7" spans="1:13" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -748,7 +760,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:13" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>2</v>
       </c>
@@ -786,7 +798,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:13" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>2</v>
       </c>
@@ -819,7 +831,7 @@
       </c>
       <c r="L9" s="10"/>
     </row>
-    <row r="10" spans="1:13" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>2</v>
       </c>
@@ -857,7 +869,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:13" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>2</v>
       </c>
@@ -890,7 +902,7 @@
       </c>
       <c r="L11" s="10"/>
     </row>
-    <row r="12" spans="1:13" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>3</v>
       </c>
@@ -928,7 +940,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:13" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>3</v>
       </c>
@@ -966,7 +978,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:13" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>3</v>
       </c>
@@ -999,7 +1011,7 @@
       </c>
       <c r="L14" s="10"/>
     </row>
-    <row r="15" spans="1:13" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>3</v>
       </c>
@@ -1037,7 +1049,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:13" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>3</v>
       </c>
@@ -1070,187 +1082,607 @@
       </c>
       <c r="L16" s="10"/>
     </row>
-    <row r="19" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-    </row>
-    <row r="20" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-    </row>
-    <row r="21" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-    </row>
-    <row r="22" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-    </row>
-    <row r="23" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-    </row>
-    <row r="24" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="18" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L18" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="M18" s="13">
+        <v>1</v>
+      </c>
+      <c r="N18" s="13">
+        <v>2</v>
+      </c>
+      <c r="O18" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="2">
+        <v>1</v>
+      </c>
+      <c r="B19" s="2">
+        <v>5</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.15827575814418399</v>
+      </c>
+      <c r="D19" s="3">
+        <v>2.3879249448083201E-9</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0.39022860405314902</v>
+      </c>
+      <c r="F19" s="3">
+        <v>503.98848207918797</v>
+      </c>
+      <c r="G19" s="3">
+        <v>5.6504618666395397E-2</v>
+      </c>
+      <c r="H19" s="3">
+        <v>3.9265906788232698E-2</v>
+      </c>
+      <c r="I19" s="3">
+        <v>1.3696922581304201</v>
+      </c>
+      <c r="J19" s="3">
+        <v>33.008734072643797</v>
+      </c>
+      <c r="L19" s="12">
+        <v>5</v>
+      </c>
+      <c r="M19" s="14">
+        <f>J19</f>
+        <v>33.008734072643797</v>
+      </c>
+      <c r="N19" s="14">
+        <f>J24</f>
+        <v>43.112971205027002</v>
+      </c>
+      <c r="O19" s="14">
+        <f>J29</f>
+        <v>54.9062998906589</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="2">
+        <v>1</v>
+      </c>
+      <c r="B20" s="2">
+        <v>10</v>
+      </c>
+      <c r="C20" s="3">
+        <v>8.7546766962356207E-2</v>
+      </c>
+      <c r="D20" s="3">
+        <v>2.44502458753337E-2</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0.22303138508175799</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0.309204676536666</v>
+      </c>
+      <c r="G20" s="3">
+        <v>4.5392277684811799E-2</v>
+      </c>
+      <c r="H20" s="3">
+        <v>1.6787245158566201E-6</v>
+      </c>
+      <c r="I20" s="3">
+        <v>0.56166381992914804</v>
+      </c>
+      <c r="J20" s="3">
+        <v>38.711057602468003</v>
+      </c>
+      <c r="L20" s="12">
+        <v>10</v>
+      </c>
+      <c r="M20" s="14">
+        <f>J20</f>
+        <v>38.711057602468003</v>
+      </c>
+      <c r="N20" s="14">
+        <f t="shared" ref="N20:N23" si="0">J25</f>
+        <v>52.755615130443203</v>
+      </c>
+      <c r="O20" s="14">
+        <f t="shared" ref="O20:O23" si="1">J30</f>
+        <v>70.604884418899303</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="2">
+        <v>1</v>
+      </c>
+      <c r="B21" s="2">
+        <v>20</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0.103712504030541</v>
+      </c>
+      <c r="D21" s="3">
+        <v>45.994984174281498</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0.44782603683072603</v>
+      </c>
+      <c r="F21" s="3">
+        <v>310.639296830663</v>
+      </c>
+      <c r="G21" s="3">
+        <v>3.3624213909445103E-2</v>
+      </c>
+      <c r="H21" s="3">
+        <v>4.1360092558262301E-5</v>
+      </c>
+      <c r="I21" s="3">
+        <v>0.53669557244817701</v>
+      </c>
+      <c r="J21" s="3">
+        <v>64.012238980091993</v>
+      </c>
+      <c r="L21" s="12">
+        <v>20</v>
+      </c>
+      <c r="M21" s="14">
+        <f t="shared" ref="M21:M23" si="2">J21</f>
+        <v>64.012238980091993</v>
+      </c>
+      <c r="N21" s="14">
+        <f t="shared" si="0"/>
+        <v>71.531258124005504</v>
+      </c>
+      <c r="O21" s="14">
+        <f t="shared" si="1"/>
+        <v>100.735029734698</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2">
+        <v>1</v>
+      </c>
+      <c r="B22" s="2">
+        <v>50</v>
+      </c>
+      <c r="C22" s="3">
+        <v>7.9999881128124603E-2</v>
+      </c>
+      <c r="D22" s="3">
+        <v>12.615708775063201</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1.30240673176306E-5</v>
+      </c>
+      <c r="F22" s="3">
+        <v>4.8504808526661103</v>
+      </c>
+      <c r="G22" s="3">
+        <v>3.2572200040363403E-2</v>
+      </c>
+      <c r="H22" s="3">
+        <v>1.6386925706611901E-2</v>
+      </c>
+      <c r="I22" s="3">
+        <v>0.56712416209923699</v>
+      </c>
+      <c r="J22" s="3">
+        <v>94.337520883365301</v>
+      </c>
+      <c r="L22" s="12">
+        <v>50</v>
+      </c>
+      <c r="M22" s="14">
+        <f t="shared" si="2"/>
+        <v>94.337520883365301</v>
+      </c>
+      <c r="N22" s="14">
+        <f t="shared" si="0"/>
+        <v>158.938225532768</v>
+      </c>
+      <c r="O22" s="14">
+        <f t="shared" si="1"/>
+        <v>195.25087067326299</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="2">
+        <v>1</v>
+      </c>
+      <c r="B23" s="2">
+        <v>70</v>
+      </c>
+      <c r="C23" s="3">
+        <v>5.7142856018037202E-2</v>
+      </c>
+      <c r="D23" s="3">
+        <v>3.3535574300585602</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1.4465113334388799E-7</v>
+      </c>
+      <c r="F23" s="3">
+        <v>213.323622416864</v>
+      </c>
+      <c r="G23" s="3">
+        <v>4.9561634297833501E-2</v>
+      </c>
+      <c r="H23" s="3">
+        <v>3.3060128673631103E-2</v>
+      </c>
+      <c r="I23" s="3">
+        <v>0.55492415772483605</v>
+      </c>
+      <c r="J23" s="3">
+        <v>131.89469646772201</v>
+      </c>
+      <c r="L23" s="12">
+        <v>70</v>
+      </c>
+      <c r="M23" s="14">
+        <f t="shared" si="2"/>
+        <v>131.89469646772201</v>
+      </c>
+      <c r="N23" s="14">
+        <f t="shared" si="0"/>
+        <v>198.01435404164999</v>
+      </c>
+      <c r="O23" s="14">
+        <f t="shared" si="1"/>
+        <v>272.97476456644699</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="2">
+        <v>2</v>
+      </c>
+      <c r="B24" s="2">
+        <v>5</v>
+      </c>
+      <c r="C24" s="4">
+        <v>0.103573974231485</v>
+      </c>
+      <c r="D24" s="4">
+        <v>0.30422228850092498</v>
+      </c>
+      <c r="E24" s="4">
+        <v>0.53151680441788296</v>
+      </c>
+      <c r="F24" s="4">
+        <v>73.974362884044297</v>
+      </c>
+      <c r="G24" s="4">
+        <v>4.4194244739570801E-2</v>
+      </c>
+      <c r="H24" s="4">
+        <v>8.2372196725553203E-9</v>
+      </c>
+      <c r="I24" s="4">
+        <v>0.53669977057168405</v>
+      </c>
+      <c r="J24" s="4">
+        <v>43.112971205027002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="2">
+        <v>2</v>
+      </c>
+      <c r="B25" s="2">
+        <v>10</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0.103668854491216</v>
+      </c>
+      <c r="D25" s="4">
+        <v>0.77951433245892898</v>
+      </c>
+      <c r="E25" s="4">
+        <v>0.53913851856647199</v>
+      </c>
+      <c r="F25" s="4">
+        <v>1.59894530889765</v>
+      </c>
+      <c r="G25" s="4">
+        <v>3.5276193371943203E-2</v>
+      </c>
+      <c r="H25" s="4">
+        <v>2.97565208690406E-10</v>
+      </c>
+      <c r="I25" s="4">
+        <v>0.53666594423400005</v>
+      </c>
+      <c r="J25" s="4">
+        <v>52.755615130443203</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="2">
+        <v>2</v>
+      </c>
+      <c r="B26" s="2">
+        <v>20</v>
+      </c>
+      <c r="C26" s="4">
+        <v>0.103102279070963</v>
+      </c>
+      <c r="D26" s="4">
+        <v>17.0331958085693</v>
+      </c>
+      <c r="E26" s="4">
+        <v>0.52500721950214801</v>
+      </c>
+      <c r="F26" s="4">
+        <v>0.29060180752591702</v>
+      </c>
+      <c r="G26" s="4">
+        <v>2.38011629209657E-2</v>
+      </c>
+      <c r="H26" s="4">
+        <v>1.7745541631509901E-7</v>
+      </c>
+      <c r="I26" s="4">
+        <v>0.53904303615868099</v>
+      </c>
+      <c r="J26" s="4">
+        <v>71.531258124005504</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="2">
+        <v>2</v>
+      </c>
+      <c r="B27" s="2">
+        <v>50</v>
+      </c>
+      <c r="C27" s="4">
+        <v>7.9999577868394303E-2</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0.12046228336555601</v>
+      </c>
+      <c r="E27" s="4">
+        <v>0.35638260544859302</v>
+      </c>
+      <c r="F27" s="4">
+        <v>37.769727734575497</v>
+      </c>
+      <c r="G27" s="4">
+        <v>5.0900979484251999E-2</v>
+      </c>
+      <c r="H27" s="4">
+        <v>1.1163057472576799E-2</v>
+      </c>
+      <c r="I27" s="4">
+        <v>0.54202567797235301</v>
+      </c>
+      <c r="J27" s="4">
+        <v>158.938225532768</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="2">
+        <v>2</v>
+      </c>
+      <c r="B28" s="2">
+        <v>70</v>
+      </c>
+      <c r="C28" s="4">
+        <v>5.7142793815441698E-2</v>
+      </c>
+      <c r="D28" s="4">
+        <v>728.12205751294596</v>
+      </c>
+      <c r="E28" s="4">
+        <v>0.23297666485778301</v>
+      </c>
+      <c r="F28" s="4">
+        <v>18.436763049296399</v>
+      </c>
+      <c r="G28" s="4">
+        <v>4.7512824464410103E-2</v>
+      </c>
+      <c r="H28" s="4">
+        <v>2.2197105782317799E-2</v>
+      </c>
+      <c r="I28" s="4">
+        <v>0.53777107232791699</v>
+      </c>
+      <c r="J28" s="4">
+        <v>198.01435404164999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="2">
+        <v>3</v>
+      </c>
+      <c r="B29" s="2">
+        <v>5</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0.18002231898212001</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0.131864972576901</v>
+      </c>
+      <c r="E29" s="3">
+        <v>1106.00583158929</v>
+      </c>
+      <c r="F29" s="3">
+        <v>0.42658535015104199</v>
+      </c>
+      <c r="G29" s="3">
+        <v>1.4250211392219899E-2</v>
+      </c>
+      <c r="H29" s="3">
+        <v>3.9033884917016704E-9</v>
+      </c>
+      <c r="I29" s="3">
+        <v>1.2767823110304299</v>
+      </c>
+      <c r="J29" s="3">
+        <v>54.9062998906589</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="2">
+        <v>3</v>
+      </c>
+      <c r="B30" s="2">
+        <v>10</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0.101743027582893</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0.91927693051577697</v>
+      </c>
+      <c r="E30" s="3">
+        <v>0.459298884944074</v>
+      </c>
+      <c r="F30" s="3">
+        <v>0.10718773294190399</v>
+      </c>
+      <c r="G30" s="3">
+        <v>3.4495246582629299E-2</v>
+      </c>
+      <c r="H30" s="3">
+        <v>1.37363093312735E-7</v>
+      </c>
+      <c r="I30" s="3">
+        <v>0.54164249740735904</v>
+      </c>
+      <c r="J30" s="3">
+        <v>70.604884418899303</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="2">
+        <v>3</v>
+      </c>
+      <c r="B31" s="2">
+        <v>20</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0.102551409588769</v>
+      </c>
+      <c r="D31" s="3">
+        <v>3.25197631859939</v>
+      </c>
+      <c r="E31" s="3">
+        <v>0.45958462412734302</v>
+      </c>
+      <c r="F31" s="3">
+        <v>123.929202702564</v>
+      </c>
+      <c r="G31" s="3">
+        <v>2.82538603658587E-2</v>
+      </c>
+      <c r="H31" s="3">
+        <v>4.8380199344964902E-9</v>
+      </c>
+      <c r="I31" s="3">
+        <v>0.54377980505008805</v>
+      </c>
+      <c r="J31" s="3">
+        <v>100.735029734698</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="2">
+        <v>3</v>
+      </c>
+      <c r="B32" s="2">
+        <v>50</v>
+      </c>
+      <c r="C32" s="3">
+        <v>7.9999936023750495E-2</v>
+      </c>
+      <c r="D32" s="3">
+        <v>7164.0577997021501</v>
+      </c>
+      <c r="E32" s="3">
+        <v>0.31204985427175502</v>
+      </c>
+      <c r="F32" s="3">
+        <v>6756.3845721351499</v>
+      </c>
+      <c r="G32" s="3">
+        <v>3.0300606552257602E-2</v>
+      </c>
+      <c r="H32" s="3">
+        <v>8.3908375158149202E-3</v>
+      </c>
+      <c r="I32" s="3">
+        <v>0.54445776061658901</v>
+      </c>
+      <c r="J32" s="3">
+        <v>195.25087067326299</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="2">
+        <v>3</v>
+      </c>
+      <c r="B33" s="2">
+        <v>70</v>
+      </c>
+      <c r="C33" s="3">
+        <v>5.7142854504348202E-2</v>
+      </c>
+      <c r="D33" s="3">
+        <v>29629.294508012299</v>
+      </c>
+      <c r="E33" s="3">
+        <v>0.171005633610428</v>
+      </c>
+      <c r="F33" s="3">
+        <v>400.49561124266597</v>
+      </c>
+      <c r="G33" s="3">
+        <v>4.1402103432587697E-2</v>
+      </c>
+      <c r="H33" s="3">
+        <v>1.5289704368861901E-2</v>
+      </c>
+      <c r="I33" s="3">
+        <v>0.54475670756904504</v>
+      </c>
+      <c r="J33" s="3">
+        <v>272.97476456644699</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="7"/>
@@ -1262,7 +1694,7 @@
       <c r="I34" s="7"/>
       <c r="J34" s="7"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
@@ -1274,7 +1706,7 @@
       <c r="I35" s="8"/>
       <c r="J35" s="8"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
@@ -1286,7 +1718,7 @@
       <c r="I36" s="8"/>
       <c r="J36" s="8"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -1298,7 +1730,7 @@
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="7"/>
@@ -1310,7 +1742,7 @@
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="7"/>
@@ -1322,7 +1754,7 @@
       <c r="I39" s="7"/>
       <c r="J39" s="7"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
       <c r="C40" s="7"/>
@@ -1334,7 +1766,7 @@
       <c r="I40" s="7"/>
       <c r="J40" s="7"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="7"/>
@@ -1346,7 +1778,7 @@
       <c r="I41" s="7"/>
       <c r="J41" s="7"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="7"/>
@@ -1358,7 +1790,7 @@
       <c r="I42" s="7"/>
       <c r="J42" s="7"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="7"/>
@@ -1370,7 +1802,7 @@
       <c r="I43" s="7"/>
       <c r="J43" s="7"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="7"/>
@@ -1382,7 +1814,7 @@
       <c r="I44" s="7"/>
       <c r="J44" s="7"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="C45" s="7"/>
@@ -1394,7 +1826,7 @@
       <c r="I45" s="7"/>
       <c r="J45" s="7"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="6"/>
       <c r="B46" s="6"/>
       <c r="C46" s="7"/>
@@ -1406,7 +1838,7 @@
       <c r="I46" s="7"/>
       <c r="J46" s="7"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
       <c r="C47" s="7"/>
@@ -1418,7 +1850,7 @@
       <c r="I47" s="7"/>
       <c r="J47" s="7"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="7"/>
@@ -1430,7 +1862,7 @@
       <c r="I48" s="7"/>
       <c r="J48" s="7"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="7"/>
@@ -1442,7 +1874,7 @@
       <c r="I49" s="7"/>
       <c r="J49" s="7"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="6"/>
       <c r="B50" s="6"/>
       <c r="C50" s="7"/>
@@ -1454,7 +1886,7 @@
       <c r="I50" s="7"/>
       <c r="J50" s="7"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="6"/>
       <c r="B51" s="6"/>
       <c r="C51" s="7"/>
@@ -1466,7 +1898,7 @@
       <c r="I51" s="7"/>
       <c r="J51" s="7"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="6"/>
       <c r="B52" s="6"/>
       <c r="C52" s="7"/>

</xml_diff>

<commit_message>
Dodanie modelu bez regulatora feedforward, dodanie plików do optymalizacji, zmiany w sprawozdaniu, nowe wykresy i nastawy, modele wyeksportowane do wersji 2016a
</commit_message>
<xml_diff>
--- a/SAIE_nastawy.xlsx
+++ b/SAIE_nastawy.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="20">
   <si>
     <t>r</t>
   </si>
@@ -72,6 +72,18 @@
   </si>
   <si>
     <t>tak</t>
+  </si>
+  <si>
+    <t>z1</t>
+  </si>
+  <si>
+    <t>z2</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>KONIEC SYM</t>
   </si>
 </sst>
 </file>
@@ -177,9 +189,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -203,6 +212,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="60% — akcent 1" xfId="1" builtinId="32"/>
@@ -486,8 +498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23:O23"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -535,10 +547,10 @@
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="M1" s="10" t="s">
         <v>14</v>
       </c>
     </row>
@@ -573,7 +585,7 @@
       <c r="J2" s="3">
         <v>68.735913474962302</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="9" t="s">
         <v>11</v>
       </c>
       <c r="M2" t="s">
@@ -611,7 +623,7 @@
       <c r="J3" s="3">
         <v>120.728202830562</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="9" t="s">
         <v>12</v>
       </c>
       <c r="M3" t="s">
@@ -649,7 +661,7 @@
       <c r="J4" s="3">
         <v>106.01931193313401</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="L4" s="9" t="s">
         <v>11</v>
       </c>
       <c r="M4" t="s">
@@ -687,7 +699,7 @@
       <c r="J5" s="3">
         <v>190.482009531355</v>
       </c>
-      <c r="L5" s="10"/>
+      <c r="L5" s="9"/>
     </row>
     <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
@@ -720,7 +732,7 @@
       <c r="J6" s="3">
         <v>262.31726493193497</v>
       </c>
-      <c r="L6" s="10"/>
+      <c r="L6" s="9"/>
     </row>
     <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
@@ -753,7 +765,7 @@
       <c r="J7" s="4">
         <v>47.7614663369976</v>
       </c>
-      <c r="L7" s="10" t="s">
+      <c r="L7" s="9" t="s">
         <v>12</v>
       </c>
       <c r="M7" t="s">
@@ -791,7 +803,7 @@
       <c r="J8" s="4">
         <v>54.6574761679651</v>
       </c>
-      <c r="L8" s="10" t="s">
+      <c r="L8" s="9" t="s">
         <v>11</v>
       </c>
       <c r="M8" t="s">
@@ -829,7 +841,7 @@
       <c r="J9" s="4">
         <v>73.950358902728496</v>
       </c>
-      <c r="L9" s="10"/>
+      <c r="L9" s="9"/>
     </row>
     <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
@@ -862,7 +874,7 @@
       <c r="J10" s="4">
         <v>414.44384161135798</v>
       </c>
-      <c r="L10" s="10" t="s">
+      <c r="L10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="M10" t="s">
@@ -900,7 +912,7 @@
       <c r="J11" s="4">
         <v>203.05709417923899</v>
       </c>
-      <c r="L11" s="10"/>
+      <c r="L11" s="9"/>
     </row>
     <row r="12" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
@@ -933,7 +945,7 @@
       <c r="J12" s="3">
         <v>57.191169414968201</v>
       </c>
-      <c r="L12" s="10" t="s">
+      <c r="L12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="M12" t="s">
@@ -971,7 +983,7 @@
       <c r="J13" s="3">
         <v>75.810460870437396</v>
       </c>
-      <c r="L13" s="10" t="s">
+      <c r="L13" s="9" t="s">
         <v>13</v>
       </c>
       <c r="M13" t="s">
@@ -1009,7 +1021,7 @@
       <c r="J14" s="3">
         <v>100.735029734698</v>
       </c>
-      <c r="L14" s="10"/>
+      <c r="L14" s="9"/>
     </row>
     <row r="15" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
@@ -1042,7 +1054,7 @@
       <c r="J15" s="3">
         <v>525.39153726010397</v>
       </c>
-      <c r="L15" s="10" t="s">
+      <c r="L15" s="9" t="s">
         <v>12</v>
       </c>
       <c r="M15" t="s">
@@ -1080,7 +1092,7 @@
       <c r="J16" s="3">
         <v>297.35180938389999</v>
       </c>
-      <c r="L16" s="10"/>
+      <c r="L16" s="9"/>
     </row>
     <row r="17" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="18" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1114,16 +1126,16 @@
       <c r="J18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L18" s="12" t="s">
+      <c r="L18" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="M18" s="13">
+      <c r="M18" s="12">
         <v>1</v>
       </c>
-      <c r="N18" s="13">
+      <c r="N18" s="12">
         <v>2</v>
       </c>
-      <c r="O18" s="13">
+      <c r="O18" s="12">
         <v>3</v>
       </c>
     </row>
@@ -1158,18 +1170,18 @@
       <c r="J19" s="3">
         <v>33.008734072643797</v>
       </c>
-      <c r="L19" s="12">
+      <c r="L19" s="11">
         <v>5</v>
       </c>
-      <c r="M19" s="14">
+      <c r="M19" s="13">
         <f>J19</f>
         <v>33.008734072643797</v>
       </c>
-      <c r="N19" s="14">
+      <c r="N19" s="13">
         <f>J24</f>
         <v>43.112971205027002</v>
       </c>
-      <c r="O19" s="14">
+      <c r="O19" s="13">
         <f>J29</f>
         <v>54.9062998906589</v>
       </c>
@@ -1205,18 +1217,18 @@
       <c r="J20" s="3">
         <v>38.711057602468003</v>
       </c>
-      <c r="L20" s="12">
+      <c r="L20" s="11">
         <v>10</v>
       </c>
-      <c r="M20" s="14">
+      <c r="M20" s="13">
         <f>J20</f>
         <v>38.711057602468003</v>
       </c>
-      <c r="N20" s="14">
+      <c r="N20" s="13">
         <f t="shared" ref="N20:N23" si="0">J25</f>
         <v>52.755615130443203</v>
       </c>
-      <c r="O20" s="14">
+      <c r="O20" s="13">
         <f t="shared" ref="O20:O23" si="1">J30</f>
         <v>70.604884418899303</v>
       </c>
@@ -1252,18 +1264,18 @@
       <c r="J21" s="3">
         <v>64.012238980091993</v>
       </c>
-      <c r="L21" s="12">
+      <c r="L21" s="11">
         <v>20</v>
       </c>
-      <c r="M21" s="14">
+      <c r="M21" s="13">
         <f t="shared" ref="M21:M23" si="2">J21</f>
         <v>64.012238980091993</v>
       </c>
-      <c r="N21" s="14">
+      <c r="N21" s="13">
         <f t="shared" si="0"/>
         <v>71.531258124005504</v>
       </c>
-      <c r="O21" s="14">
+      <c r="O21" s="13">
         <f t="shared" si="1"/>
         <v>100.735029734698</v>
       </c>
@@ -1299,18 +1311,18 @@
       <c r="J22" s="3">
         <v>94.337520883365301</v>
       </c>
-      <c r="L22" s="12">
+      <c r="L22" s="11">
         <v>50</v>
       </c>
-      <c r="M22" s="14">
+      <c r="M22" s="13">
         <f t="shared" si="2"/>
         <v>94.337520883365301</v>
       </c>
-      <c r="N22" s="14">
+      <c r="N22" s="13">
         <f t="shared" si="0"/>
         <v>158.938225532768</v>
       </c>
-      <c r="O22" s="14">
+      <c r="O22" s="13">
         <f t="shared" si="1"/>
         <v>195.25087067326299</v>
       </c>
@@ -1346,18 +1358,18 @@
       <c r="J23" s="3">
         <v>131.89469646772201</v>
       </c>
-      <c r="L23" s="12">
+      <c r="L23" s="11">
         <v>70</v>
       </c>
-      <c r="M23" s="14">
+      <c r="M23" s="13">
         <f t="shared" si="2"/>
         <v>131.89469646772201</v>
       </c>
-      <c r="N23" s="14">
+      <c r="N23" s="13">
         <f t="shared" si="0"/>
         <v>198.01435404164999</v>
       </c>
-      <c r="O23" s="14">
+      <c r="O23" s="13">
         <f t="shared" si="1"/>
         <v>272.97476456644699</v>
       </c>
@@ -1553,6 +1565,10 @@
       <c r="J29" s="3">
         <v>54.9062998906589</v>
       </c>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
     </row>
     <row r="30" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
@@ -1682,233 +1698,311 @@
         <v>272.97476456644699</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
-      <c r="J34" s="7"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
-      <c r="I37" s="5"/>
-      <c r="J37" s="5"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="7"/>
+    <row r="34" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+    </row>
+    <row r="35" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="2">
+        <v>2</v>
+      </c>
+      <c r="B36" s="2">
+        <v>20</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0</v>
+      </c>
+      <c r="D36" s="2">
+        <v>2.3879249448083201E-9</v>
+      </c>
+      <c r="E36" s="14">
+        <v>0.17249999999999999</v>
+      </c>
+      <c r="F36" s="14">
+        <v>7.4200000000000002E-2</v>
+      </c>
+      <c r="G36" s="14">
+        <v>9.2999999999999992E-3</v>
+      </c>
+      <c r="H36" s="14">
+        <v>62.927092484920202</v>
+      </c>
+      <c r="J36" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="2">
+        <v>2</v>
+      </c>
+      <c r="B37" s="2">
+        <v>0</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0</v>
+      </c>
+      <c r="D37" s="2">
+        <v>1</v>
+      </c>
+      <c r="E37" s="3">
+        <v>5.4818185856768604</v>
+      </c>
+      <c r="F37" s="3">
+        <v>2.3818046946299098</v>
+      </c>
+      <c r="G37" s="3">
+        <v>2.95632604402211E-4</v>
+      </c>
+      <c r="H37" s="3">
+        <v>30.538560091686399</v>
+      </c>
+      <c r="J37" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="2">
+        <v>2</v>
+      </c>
+      <c r="B38" s="2">
+        <v>0</v>
+      </c>
+      <c r="C38" s="2">
+        <v>1</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="2">
+        <v>2</v>
+      </c>
+      <c r="B39" s="2">
+        <v>0</v>
+      </c>
+      <c r="C39" s="2">
+        <v>1</v>
+      </c>
+      <c r="D39" s="2">
+        <v>1</v>
+      </c>
+      <c r="E39" s="3">
+        <v>1.7981</v>
+      </c>
+      <c r="F39" s="3">
+        <v>0.39550000000000002</v>
+      </c>
+      <c r="G39" s="3">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="H39" s="3">
+        <v>309.03868452198702</v>
+      </c>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="7"/>
-      <c r="J40" s="7"/>
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A41" s="6"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7"/>
-      <c r="I41" s="7"/>
-      <c r="J41" s="7"/>
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42" s="6"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="7"/>
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" s="6"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
-      <c r="I43" s="7"/>
-      <c r="J43" s="7"/>
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="6"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A44" s="6"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="7"/>
-      <c r="I44" s="7"/>
-      <c r="J44" s="7"/>
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="6"/>
+      <c r="J44" s="6"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" s="6"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="7"/>
-      <c r="I45" s="7"/>
-      <c r="J45" s="7"/>
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="6"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" s="6"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="7"/>
-      <c r="I46" s="7"/>
-      <c r="J46" s="7"/>
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="6"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A47" s="6"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="7"/>
-      <c r="I47" s="7"/>
-      <c r="J47" s="7"/>
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="6"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A48" s="6"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7"/>
-      <c r="G48" s="7"/>
-      <c r="H48" s="7"/>
-      <c r="I48" s="7"/>
-      <c r="J48" s="7"/>
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="6"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A49" s="6"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="7"/>
-      <c r="G49" s="7"/>
-      <c r="H49" s="7"/>
-      <c r="I49" s="7"/>
-      <c r="J49" s="7"/>
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="6"/>
+      <c r="J49" s="6"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A50" s="6"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
-      <c r="G50" s="7"/>
-      <c r="H50" s="7"/>
-      <c r="I50" s="7"/>
-      <c r="J50" s="7"/>
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="6"/>
+      <c r="J50" s="6"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A51" s="6"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="7"/>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7"/>
-      <c r="F51" s="7"/>
-      <c r="G51" s="7"/>
-      <c r="H51" s="7"/>
-      <c r="I51" s="7"/>
-      <c r="J51" s="7"/>
+      <c r="A51" s="5"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="6"/>
+      <c r="J51" s="6"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A52" s="6"/>
-      <c r="B52" s="6"/>
-      <c r="C52" s="7"/>
-      <c r="D52" s="7"/>
-      <c r="E52" s="7"/>
-      <c r="F52" s="7"/>
-      <c r="G52" s="7"/>
-      <c r="H52" s="7"/>
-      <c r="I52" s="7"/>
-      <c r="J52" s="7"/>
+      <c r="A52" s="5"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>